<commit_message>
Finished Steam and Reddit game list...
</commit_message>
<xml_diff>
--- a/Similar Games.xlsx
+++ b/Similar Games.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="49">
   <si>
     <t>Game</t>
   </si>
@@ -143,16 +143,34 @@
     <t>Time Machine VR</t>
   </si>
   <si>
-    <t>https://www.reddit.com/r/patientgamers/comments/3xm37s/games_with_time_controltime_manipulation_embedded/</t>
-  </si>
-  <si>
     <t>http://www.mobygames.com/game-group/theme-time-manipulation/offset,0/so,1a/</t>
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/List_of_games_containing_time_travel#Video_games</t>
   </si>
   <si>
-    <t>http://store.steampowered.com/tag/en/Time%20Manipulation/#p=0&amp;tab=NewReleases</t>
+    <t>Space Fuss</t>
+  </si>
+  <si>
+    <t>Sumoman</t>
+  </si>
+  <si>
+    <t>The Sexy Brutale</t>
+  </si>
+  <si>
+    <t>Mystery</t>
+  </si>
+  <si>
+    <t>Time Recoil</t>
+  </si>
+  <si>
+    <t>Puzzle-Platformer</t>
+  </si>
+  <si>
+    <t>Thinking with Time Machines</t>
+  </si>
+  <si>
+    <t>Desktop only!</t>
   </si>
 </sst>
 </file>
@@ -211,55 +229,331 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike/>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
+  <dxfs count="49">
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFFFF"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color theme="0"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -304,8 +598,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D21" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:D21"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D27" totalsRowShown="0" headerRowDxfId="48">
+  <autoFilter ref="A1:D27"/>
+  <sortState ref="A2:D27">
+    <sortCondition sortBy="fontColor" ref="A1:A27" dxfId="1"/>
+  </sortState>
   <tableColumns count="4">
     <tableColumn id="1" name="Game"/>
     <tableColumn id="2" name="2D/3D"/>
@@ -579,7 +876,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
@@ -605,6 +902,9 @@
       <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -625,66 +925,75 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
       <c r="I3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>18</v>
+      <c r="A4" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
       </c>
       <c r="I4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
+      <c r="A5" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>32</v>
       </c>
       <c r="I5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>19</v>
+      <c r="A6" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
       </c>
       <c r="I6" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>21</v>
+      <c r="A7" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -698,33 +1007,27 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="I8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>30</v>
+      <c r="A9" t="s">
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
+        <v>6</v>
       </c>
       <c r="I9" t="s">
         <v>12</v>
@@ -732,99 +1035,114 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="I10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>28</v>
+      <c r="A11" t="s">
+        <v>45</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>27</v>
+      <c r="A12" t="s">
+        <v>16</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
       </c>
       <c r="I12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>26</v>
+      <c r="A13" t="s">
+        <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>24</v>
+      <c r="A15" t="s">
+        <v>35</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="I16" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -832,42 +1150,112 @@
       <c r="C17" t="s">
         <v>6</v>
       </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
       <c r="I17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" t="s">
-        <v>42</v>
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:D21">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A2:D27">
+    <cfRule type="expression" dxfId="13" priority="4">
+      <formula>$D2="Shooter"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>$B2="2D"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="3">
+      <formula>$D2="Simulation"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="2">
+      <formula>$D2="Real time strategy"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>